<commit_message>
improve second example analysis
</commit_message>
<xml_diff>
--- a/exampleAnalysis2/MassProfiles.xlsx
+++ b/exampleAnalysis2/MassProfiles.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="33">
   <si>
     <t>year</t>
   </si>
@@ -99,28 +99,34 @@
     <t>Gresham</t>
   </si>
   <si>
-    <t>baseline_metroApproximation</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
-    <t>based on Metro's total and Gresham's population as a portion of Metro's</t>
-  </si>
-  <si>
-    <t>based on dirthugger document</t>
-  </si>
-  <si>
-    <t>alternative_all_to_dirthugger</t>
-  </si>
-  <si>
-    <t>alternative_6pt5</t>
-  </si>
-  <si>
-    <t>based on idea that food waste is 6.5% of mixed yard debris/food waste</t>
-  </si>
-  <si>
     <t>based on idea that food waste is 6.5% of mixed yard debris/food waste (see metro waste study)</t>
+  </si>
+  <si>
+    <t>based on Metro's total and Gresham's population as a portion of Metro's, adjusted to 9000 tons yard debris standard</t>
+  </si>
+  <si>
+    <t>compost_1000t</t>
+  </si>
+  <si>
+    <t>compost_6pt5pct</t>
+  </si>
+  <si>
+    <t>reduce_fw_10pct</t>
+  </si>
+  <si>
+    <t>reduce_fw_05pct</t>
+  </si>
+  <si>
+    <t>based on projection that 1000 tons of food waste could be composted</t>
+  </si>
+  <si>
+    <t>baseline, but with 5 percent less food waste</t>
+  </si>
+  <si>
+    <t>baseline, but with 10 percent less food waste</t>
   </si>
 </sst>
 </file>
@@ -462,23 +468,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.88671875" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" customWidth="1"/>
     <col min="2" max="2" width="11.88671875" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8" customWidth="1"/>
+    <col min="4" max="5" width="14.109375" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
@@ -491,19 +497,22 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
@@ -514,20 +523,23 @@
       <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1">
-        <f>SUM('metro mass profile 2018'!E2:E6)*greshamMetroRatio</f>
-        <v>15699.7999477345</v>
-      </c>
-      <c r="F2">
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1">
+        <f>ROUND(SUM('metro mass profile 2018'!E2:E6)*greshamMetroRatio/2.04722,0)</f>
+        <v>7669</v>
+      </c>
+      <c r="G2">
         <v>178</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
@@ -538,20 +550,23 @@
       <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="1">
-        <f>SUM('metro mass profile 2018'!E7:E11)*greshamMetroRatio</f>
-        <v>18424.563307310662</v>
-      </c>
-      <c r="F3">
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1">
+        <f>ROUND(SUM('metro mass profile 2018'!E7:E11)*greshamMetroRatio/2.047222,0)</f>
+        <v>9000</v>
+      </c>
+      <c r="G3">
         <v>5</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
@@ -560,65 +575,75 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="1">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1">
         <v>1000</v>
       </c>
-      <c r="F4">
-        <v>178</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="G4">
+        <v>78</v>
+      </c>
+      <c r="H4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>17</v>
       </c>
       <c r="B5" t="s">
         <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="1">
-        <v>9000</v>
-      </c>
-      <c r="F5">
-        <v>5</v>
-      </c>
-      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1">
+        <f>F2-F4</f>
+        <v>6669</v>
+      </c>
+      <c r="G5">
+        <v>178</v>
+      </c>
+      <c r="H5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>27</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="1">
-        <v>1000</v>
-      </c>
-      <c r="F6">
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1">
+        <v>9000</v>
+      </c>
+      <c r="G6">
         <v>78</v>
       </c>
-      <c r="G6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -626,24 +651,28 @@
         <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="1">
-        <v>9000</v>
-      </c>
-      <c r="F7">
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1">
+        <f>F9*0.065</f>
+        <v>585</v>
+      </c>
+      <c r="G7">
         <v>78</v>
       </c>
-      <c r="G7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
         <v>22</v>
@@ -652,22 +681,25 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="1">
-        <f>E9*0.065</f>
-        <v>585</v>
-      </c>
-      <c r="F8">
-        <v>78</v>
-      </c>
-      <c r="G8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="1">
+        <f>F2-F7</f>
+        <v>7084</v>
+      </c>
+      <c r="G8">
+        <v>178</v>
+      </c>
+      <c r="H8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
@@ -678,14 +710,125 @@
       <c r="D9" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="1">
         <v>9000</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>78</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="1">
+        <f>F2*0.95</f>
+        <v>7285.5499999999993</v>
+      </c>
+      <c r="G10">
+        <v>178</v>
+      </c>
+      <c r="H10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1">
+        <f>F3</f>
+        <v>9000</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="H11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="1">
+        <f>F2*0.9</f>
+        <v>6902.1</v>
+      </c>
+      <c r="G12">
+        <v>178</v>
+      </c>
+      <c r="H12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="1">
+        <f>F3</f>
+        <v>9000</v>
+      </c>
+      <c r="G13">
+        <v>5</v>
+      </c>
+      <c r="H13" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improve example analysis so it's about Anytown
</commit_message>
<xml_diff>
--- a/exampleAnalysis2/MassProfiles.xlsx
+++ b/exampleAnalysis2/MassProfiles.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="34">
   <si>
     <t>year</t>
   </si>
@@ -108,25 +108,28 @@
     <t>based on Metro's total and Gresham's population as a portion of Metro's, adjusted to 9000 tons yard debris standard</t>
   </si>
   <si>
-    <t>compost_1000t</t>
-  </si>
-  <si>
-    <t>compost_6pt5pct</t>
-  </si>
-  <si>
-    <t>reduce_fw_10pct</t>
-  </si>
-  <si>
-    <t>reduce_fw_05pct</t>
-  </si>
-  <si>
     <t>based on projection that 1000 tons of food waste could be composted</t>
   </si>
   <si>
-    <t>baseline, but with 5 percent less food waste</t>
-  </si>
-  <si>
-    <t>baseline, but with 10 percent less food waste</t>
+    <t>baseline, but with 3 percent less food waste</t>
+  </si>
+  <si>
+    <t>baseline, but with 6 percent less food waste generated</t>
+  </si>
+  <si>
+    <t>reduceFW03</t>
+  </si>
+  <si>
+    <t>reduceFW06</t>
+  </si>
+  <si>
+    <t>reductFW06</t>
+  </si>
+  <si>
+    <t>compostFW1000</t>
+  </si>
+  <si>
+    <t>compostFW585</t>
   </si>
 </sst>
 </file>
@@ -471,7 +474,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection sqref="A1:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -566,7 +569,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
@@ -587,12 +590,12 @@
         <v>78</v>
       </c>
       <c r="H4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
         <v>22</v>
@@ -614,12 +617,12 @@
         <v>178</v>
       </c>
       <c r="H5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
@@ -640,12 +643,12 @@
         <v>78</v>
       </c>
       <c r="H6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
         <v>22</v>
@@ -672,7 +675,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>22</v>
@@ -699,7 +702,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
@@ -740,14 +743,14 @@
         <v>12</v>
       </c>
       <c r="F10" s="1">
-        <f>F2*0.95</f>
-        <v>7285.5499999999993</v>
+        <f>F2*0.97</f>
+        <v>7438.9299999999994</v>
       </c>
       <c r="G10">
         <v>178</v>
       </c>
       <c r="H10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -774,12 +777,12 @@
         <v>5</v>
       </c>
       <c r="H11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
         <v>22</v>
@@ -794,19 +797,19 @@
         <v>12</v>
       </c>
       <c r="F12" s="1">
-        <f>F2*0.9</f>
-        <v>6902.1</v>
+        <f>F2*0.94</f>
+        <v>7208.86</v>
       </c>
       <c r="G12">
         <v>178</v>
       </c>
       <c r="H12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
@@ -828,7 +831,7 @@
         <v>5</v>
       </c>
       <c r="H13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -842,7 +845,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>